<commit_message>
Adição do arquivo README ao projeto
Realização de algumas edições nos dashboards
</commit_message>
<xml_diff>
--- a/assets/planilhas/Book-Catalogue.xlsx
+++ b/assets/planilhas/Book-Catalogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delab\OneDrive\Área de Trabalho\Planilhas-Excel\assets\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391D18BE-ECAE-447B-B94D-30EC9E03B2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DD9D96-4794-49B6-88B2-6079C9CE3F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="996" yWindow="-108" windowWidth="22152" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="996" yWindow="-108" windowWidth="22152" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogue" sheetId="1" r:id="rId1"/>
@@ -1155,12 +1155,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1197,6 +1191,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1209,67 +1206,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF7E8FF2"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Segoe UI Semibold"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF6B71F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1577,10 +1521,66 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF7E8FF2"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Segoe UI Semibold"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF6B71F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -6665,20 +6665,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD9279C4-4C61-46B0-9F0F-090C46869F26}" name="Tabela1" displayName="Tabela1" ref="B6:L36" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="14" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD9279C4-4C61-46B0-9F0F-090C46869F26}" name="Tabela1" displayName="Tabela1" ref="B6:L36" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
   <autoFilter ref="B6:L36" xr:uid="{CD9279C4-4C61-46B0-9F0F-090C46869F26}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{0426D1FE-FA03-42DA-8A8A-026073E2AF16}" name="ISBN" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{8A78A841-8173-4E12-8B81-45680DA8729A}" name="Título" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{3E6089A2-3A47-4E96-AFFD-906515382165}" name="Gênero" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{1385160A-26D6-4ED6-A4E9-E9840756FB75}" name="Autoria" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{C4B21762-A258-435A-983F-ACA44734A88C}" name="Editora" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{5A7C7A14-20D6-4CC7-A73F-C590972A260A}" name="Publicação" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{A831E45C-BD76-4B5E-BF27-B7283897E4E1}" name="Páginas" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{8A8CC8AF-51D2-4B13-85F7-F5AB6A51E870}" name="Modelo" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{4E613AAA-4AF2-4CA9-9C23-58C2BC3217B0}" name="Status" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{EB4C3150-9503-4B82-9E0B-84CBD012D27C}" name="Capa" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{42484302-6F79-4F17-9DD3-69E8C06311B9}" name="Nota" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{0426D1FE-FA03-42DA-8A8A-026073E2AF16}" name="ISBN" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{8A78A841-8173-4E12-8B81-45680DA8729A}" name="Título" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{3E6089A2-3A47-4E96-AFFD-906515382165}" name="Gênero" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{1385160A-26D6-4ED6-A4E9-E9840756FB75}" name="Autoria" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{C4B21762-A258-435A-983F-ACA44734A88C}" name="Editora" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{5A7C7A14-20D6-4CC7-A73F-C590972A260A}" name="Publicação" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{A831E45C-BD76-4B5E-BF27-B7283897E4E1}" name="Páginas" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{8A8CC8AF-51D2-4B13-85F7-F5AB6A51E870}" name="Modelo" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{4E613AAA-4AF2-4CA9-9C23-58C2BC3217B0}" name="Status" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{EB4C3150-9503-4B82-9E0B-84CBD012D27C}" name="Capa" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{42484302-6F79-4F17-9DD3-69E8C06311B9}" name="Nota" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6982,11 +6982,11 @@
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="8"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="34"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="32"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6996,11 +6996,11 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
       <c r="I2" s="8"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="34"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="32"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -7010,11 +7010,11 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
       <c r="I3" s="8"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="34"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="32"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -7024,11 +7024,11 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
       <c r="I4" s="8"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="34"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="32"/>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -7085,37 +7085,37 @@
     </row>
     <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="35" t="s">
         <v>25</v>
       </c>
       <c r="G7" s="10">
         <v>2002</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="36">
         <v>208</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I7" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="37" t="s">
+      <c r="J7" s="35" t="s">
         <v>18</v>
       </c>
       <c r="K7" s="10" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="L7" s="39">
+      <c r="L7" s="37">
         <v>5</v>
       </c>
       <c r="M7" s="1"/>
@@ -8221,7 +8221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{572947D5-7A58-40BF-AFCF-CE310F25EDAD}">
   <dimension ref="B1:M22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -8238,38 +8238,38 @@
     </row>
     <row r="3" spans="2:2" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="9:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I17" s="31" t="e" vm="31">
+      <c r="I17" s="43" t="e" vm="31">
         <f>VLOOKUP(Operations!J7, Catalogue!C7:L36, 9, FALSE)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K17" s="31" t="e" vm="32">
+      <c r="K17" s="43" t="e" vm="32">
         <f>VLOOKUP(Operations!J8, Catalogue!C7:L36, 9, FALSE)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M17" s="31" t="e" vm="33">
+      <c r="M17" s="43" t="e" vm="33">
         <f>VLOOKUP(Operations!J9, Catalogue!C7:L36, 9, FALSE)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" spans="9:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="M18" s="31"/>
+      <c r="I18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="M18" s="43"/>
     </row>
     <row r="19" spans="9:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="M19" s="31"/>
+      <c r="I19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="M19" s="43"/>
     </row>
     <row r="20" spans="9:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="M20" s="31"/>
+      <c r="I20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="M20" s="43"/>
     </row>
     <row r="21" spans="9:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="M21" s="31"/>
+      <c r="I21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="M21" s="43"/>
     </row>
     <row r="22" spans="9:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I22" s="6"/>
@@ -8408,7 +8408,7 @@
       <c r="B6" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="40"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="30" t="s">
         <v>6</v>
       </c>
@@ -8423,10 +8423,10 @@
         <v>122</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="41" t="s">
+      <c r="J6" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="K6" s="41" t="s">
+      <c r="K6" s="39" t="s">
         <v>6</v>
       </c>
       <c r="L6" s="3"/>
@@ -8448,16 +8448,16 @@
         <f t="array" ref="D7:D22">SUMIFS(Tabela1[Páginas], Tabela1[Autoria],_xlfn.ANCHORARRAY( E7))</f>
         <v>208</v>
       </c>
-      <c r="E7" s="42" t="str" cm="1">
+      <c r="E7" s="40" t="str" cm="1">
         <f t="array" ref="E7:E22">_xlfn.UNIQUE(Tabela1[Autoria])</f>
         <v>Neil Gaiman</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="42" t="str" cm="1">
+      <c r="G7" s="40" t="str" cm="1">
         <f t="array" ref="G7:G19">_xlfn.UNIQUE(Tabela1[Editora])</f>
         <v>Harper Collins</v>
       </c>
-      <c r="H7" s="42" cm="1">
+      <c r="H7" s="40" cm="1">
         <f t="array" ref="H7:H19">COUNTIF(Tabela1[Editora],_xlfn.ANCHORARRAY( G7))</f>
         <v>6</v>
       </c>
@@ -8466,7 +8466,7 @@
         <f t="array" ref="J7">_xlfn._xlws.FILTER(Tabela1[Título], Tabela1[Páginas]=LARGE(Tabela1[Páginas], 1))</f>
         <v>Harry Potter: e a ordem da Fênix</v>
       </c>
-      <c r="K7" s="43" t="str">
+      <c r="K7" s="41" t="str">
         <f>LARGE(Tabela1[Páginas], 1)&amp;" pág."</f>
         <v>876 pág.</v>
       </c>
@@ -8501,7 +8501,7 @@
         <f t="array" ref="J8">_xlfn._xlws.FILTER(Tabela1[Título], Tabela1[Páginas]=LARGE(Tabela1[Páginas], 2))</f>
         <v>Harry Potter: e as relíquias da morte</v>
       </c>
-      <c r="K8" s="43" t="str">
+      <c r="K8" s="41" t="str">
         <f>LARGE(Tabela1[Páginas], 2)&amp;" pág."</f>
         <v>784 pág.</v>
       </c>
@@ -8532,11 +8532,11 @@
         <v>1</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="44" t="str" cm="1">
+      <c r="J9" s="42" t="str" cm="1">
         <f t="array" ref="J9">_xlfn._xlws.FILTER(Tabela1[Título], Tabela1[Páginas]=LARGE(Tabela1[Páginas], 3))</f>
         <v>As crônicas de Narnia</v>
       </c>
-      <c r="K9" s="43" t="str">
+      <c r="K9" s="41" t="str">
         <f>LARGE(Tabela1[Páginas], 3)&amp;" pág."</f>
         <v>752 pág.</v>
       </c>
@@ -8596,10 +8596,10 @@
         <v>1</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="45" t="s">
+      <c r="J11" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="K11" s="46"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -8627,11 +8627,11 @@
         <v>1</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="47" t="str">
+      <c r="J12" s="46" t="str">
         <f>VLOOKUP(LARGE(_xlfn.ANCHORARRAY(D7), 1), $D$7:$E$22, 2, FALSE)&amp;", com "&amp;LARGE(_xlfn.ANCHORARRAY(D7), 1)&amp;" páginas"</f>
         <v>J.K. Rowling, com 3859 páginas</v>
       </c>
-      <c r="K12" s="48"/>
+      <c r="K12" s="47"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -8688,10 +8688,10 @@
         <v>1</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="45" t="s">
+      <c r="J14" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="K14" s="46"/>
+      <c r="K14" s="45"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -8701,7 +8701,7 @@
     </row>
     <row r="15" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="42" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="3"/>
@@ -8719,11 +8719,11 @@
         <v>1</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="47" t="str">
+      <c r="J15" s="46" t="str">
         <f>SUMIFS(Tabela1[Páginas], Tabela1[Status], "concluído")&amp;" páginas"</f>
         <v>6972 páginas</v>
       </c>
-      <c r="K15" s="48"/>
+      <c r="K15" s="47"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
@@ -8827,10 +8827,10 @@
         <v>H.P. Lovecraft</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="44" t="str">
+      <c r="G19" s="42" t="str">
         <v>Pé da Letra</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="42">
         <v>2</v>
       </c>
       <c r="I19" s="3"/>
@@ -8881,10 +8881,10 @@
         <v>Robert L. Steverson</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="45" t="s">
+      <c r="G21" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="H21" s="46"/>
+      <c r="H21" s="45"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -8897,22 +8897,22 @@
     </row>
     <row r="22" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="29">
         <v>2400</v>
       </c>
-      <c r="E22" s="44" t="str">
+      <c r="E22" s="42" t="str">
         <v>J.R.R. Tolkien</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="47" t="str">
+      <c r="G22" s="46" t="str">
         <f>COUNTA(Catalogue!$C$7:$C$36)&amp;" volumes"</f>
         <v>30 volumes</v>
       </c>
-      <c r="H22" s="48"/>
+      <c r="H22" s="47"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -9005,7 +9005,7 @@
     </row>
     <row r="27" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="42" t="s">
         <v>97</v>
       </c>
       <c r="C27" s="3"/>
@@ -9048,7 +9048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56ECCED4-D617-4FDA-AEA2-A516CE707CA8}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -9069,33 +9069,33 @@
       <c r="B6" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="32" t="e" vm="34">
+      <c r="E6" s="48" t="e" vm="34">
         <f>VLOOKUP(B7,Catalogue!$B$7:$L$1048576,10,FALSE)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
@@ -9105,9 +9105,9 @@
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
@@ -9117,9 +9117,9 @@
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23"/>
@@ -9129,9 +9129,9 @@
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="23"/>
@@ -9141,47 +9141,47 @@
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>